<commit_message>
added lat longs * quote all text fields
</commit_message>
<xml_diff>
--- a/dam_csv/map_dams.xlsx
+++ b/dam_csv/map_dams.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">DamId</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">pk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dam_ID</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -52,31 +55,55 @@
     <t xml:space="preserve">Year of Installation</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4190</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ripogenus Dam</t>
   </si>
   <si>
     <t xml:space="preserve">S</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4679</t>
+  </si>
+  <si>
     <t xml:space="preserve">Medway Dam</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4180</t>
+  </si>
+  <si>
     <t xml:space="preserve">Millonocket/Quakish Dam</t>
   </si>
   <si>
     <t xml:space="preserve">M</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4179</t>
+  </si>
+  <si>
     <t xml:space="preserve">Millonocket Lake Dam</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4178</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dolby Dam</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4181</t>
+  </si>
+  <si>
     <t xml:space="preserve">North Twin Dam</t>
   </si>
   <si>
+    <t xml:space="preserve">DamID_4677</t>
+  </si>
+  <si>
     <t xml:space="preserve">East Millonocket Dam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DamID_4702</t>
   </si>
   <si>
     <t xml:space="preserve">West Enfield Dam</t>
@@ -95,6 +122,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,8 +182,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -180,30 +212,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.23"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="37.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="27.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="37.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
@@ -230,30 +262,43 @@
       <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>45.88144746</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>-69.17626004</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>2572</v>
       </c>
-      <c r="F2" s="1" t="b">
+      <c r="G2" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="n">
         <v>37.5</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="J2" s="0" t="n">
         <v>234</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <v>1916</v>
       </c>
     </row>
@@ -261,25 +306,35 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>45.60743512</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>-68.54566603</v>
+      </c>
+      <c r="F3" s="0" t="n">
         <v>2666</v>
       </c>
-      <c r="F3" s="1" t="b">
+      <c r="G3" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="n">
         <v>3.4</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="J3" s="0" t="n">
         <v>28.1</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="K3" s="0" t="n">
         <v>1922</v>
       </c>
     </row>
@@ -287,25 +342,35 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="0" t="n">
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>45.63856608</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>-68.72847936</v>
+      </c>
+      <c r="F4" s="0" t="n">
         <v>2458</v>
       </c>
-      <c r="F4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="J4" s="0" t="n">
         <v>203.3</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="K4" s="0" t="n">
         <v>1900</v>
       </c>
     </row>
@@ -313,25 +378,35 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="0" t="n">
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45.74234707</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>-68.73347543</v>
+      </c>
+      <c r="F5" s="0" t="n">
         <v>2458</v>
       </c>
-      <c r="F5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>0</v>
+      <c r="G5" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>1883</v>
       </c>
     </row>
@@ -339,25 +414,35 @@
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>45.6326293</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>-68.60699086</v>
+      </c>
+      <c r="F6" s="0" t="n">
         <v>2458</v>
       </c>
-      <c r="F6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="G6" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="0" t="n">
         <v>20.9</v>
       </c>
-      <c r="I6" s="0" t="n">
+      <c r="J6" s="0" t="n">
         <v>98.1</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="K6" s="0" t="n">
         <v>1907</v>
       </c>
     </row>
@@ -365,25 +450,35 @@
       <c r="A7" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="0" t="n">
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>45.63470712</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>-68.78039159</v>
+      </c>
+      <c r="F7" s="0" t="n">
         <v>2458</v>
       </c>
-      <c r="F7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="G7" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="I7" s="0" t="n">
+      <c r="J7" s="0" t="n">
         <v>47.3</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="K7" s="0" t="n">
         <v>1846</v>
       </c>
     </row>
@@ -391,25 +486,35 @@
       <c r="A8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>45.62091833</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>-68.57601026</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2458</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="0" t="n">
-        <v>2458</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="I8" s="0" t="n">
         <v>6.9</v>
       </c>
-      <c r="I8" s="0" t="n">
+      <c r="J8" s="0" t="n">
         <v>37.7</v>
       </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="0" t="n">
         <v>1906</v>
       </c>
     </row>
@@ -417,25 +522,35 @@
       <c r="A9" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>45.25014604</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>-68.64874868</v>
+      </c>
+      <c r="F9" s="0" t="n">
         <v>2600</v>
       </c>
-      <c r="F9" s="1" t="b">
+      <c r="G9" s="2" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="0" t="s">
         <v>13</v>
       </c>
       <c r="I9" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" s="0" t="n">
         <v>91.8</v>
       </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="0" t="n">
         <v>1894</v>
       </c>
     </row>

</xml_diff>